<commit_message>
added daily measurment series notification
added daily measurment series notification
</commit_message>
<xml_diff>
--- a/excel/message_details/message_details_MeasurementSeriesNotificationMonthly.xlsx
+++ b/excel/message_details/message_details_MeasurementSeriesNotificationMonthly.xlsx
@@ -10,7 +10,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="decompressed cases" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -75,16 +75,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -500,24 +494,24 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>XML ELEMENT PATH</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>DEFAULT VALUES</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Error Message 1</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/EDSNBusinessDocumentHeader/ContentHash</t>
         </is>
@@ -534,7 +528,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/EDSNBusinessDocumentHeader/ConversationID</t>
         </is>
@@ -551,7 +545,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/EDSNBusinessDocumentHeader/CorrelationID</t>
         </is>
@@ -568,7 +562,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/EDSNBusinessDocumentHeader/CreationTimestamp</t>
         </is>
@@ -585,7 +579,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/EDSNBusinessDocumentHeader/DocumentID</t>
         </is>
@@ -602,7 +596,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/EDSNBusinessDocumentHeader/ExpiresAt</t>
         </is>
@@ -619,7 +613,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="inlineStr">
+      <c r="A8" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/EDSNBusinessDocumentHeader/MessageID</t>
         </is>
@@ -636,7 +630,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="inlineStr">
+      <c r="A9" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/EDSNBusinessDocumentHeader/ProcessTypeID</t>
         </is>
@@ -653,7 +647,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="inlineStr">
+      <c r="A10" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/EDSNBusinessDocumentHeader/RepeatedRequest</t>
         </is>
@@ -670,7 +664,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="inlineStr">
+      <c r="A11" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/EDSNBusinessDocumentHeader/TestRequest</t>
         </is>
@@ -687,7 +681,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="inlineStr">
+      <c r="A12" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/EDSNBusinessDocumentHeader/Destination/Receiver/Authority</t>
         </is>
@@ -704,7 +698,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="4" t="inlineStr">
+      <c r="A13" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/EDSNBusinessDocumentHeader/Destination/Receiver/ContactTypeIdentifier</t>
         </is>
@@ -721,7 +715,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="inlineStr">
+      <c r="A14" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/EDSNBusinessDocumentHeader/Destination/Receiver/ReceiverID</t>
         </is>
@@ -738,7 +732,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="4" t="inlineStr">
+      <c r="A15" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/EDSNBusinessDocumentHeader/Destination/Service/ServiceMethod</t>
         </is>
@@ -755,7 +749,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="4" t="inlineStr">
+      <c r="A16" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/EDSNBusinessDocumentHeader/Destination/Service/ServiceName</t>
         </is>
@@ -772,7 +766,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="4" t="inlineStr">
+      <c r="A17" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/EDSNBusinessDocumentHeader/Manifest/NumberofItems</t>
         </is>
@@ -789,7 +783,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="inlineStr">
+      <c r="A18" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/EDSNBusinessDocumentHeader/Manifest/ManifestItem/Description</t>
         </is>
@@ -806,7 +800,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="4" t="inlineStr">
+      <c r="A19" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/EDSNBusinessDocumentHeader/Manifest/ManifestItem/LanguageCode</t>
         </is>
@@ -823,7 +817,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="4" t="inlineStr">
+      <c r="A20" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/EDSNBusinessDocumentHeader/Manifest/ManifestItem/MimeTypeQualifierCode</t>
         </is>
@@ -840,7 +834,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="4" t="inlineStr">
+      <c r="A21" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/EDSNBusinessDocumentHeader/Manifest/ManifestItem/UniformResourceIdentifier</t>
         </is>
@@ -857,7 +851,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="4" t="inlineStr">
+      <c r="A22" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/EDSNBusinessDocumentHeader/Source/Authority</t>
         </is>
@@ -874,7 +868,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="4" t="inlineStr">
+      <c r="A23" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/EDSNBusinessDocumentHeader/Source/ContactTypeIdentifier</t>
         </is>
@@ -891,7 +885,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="4" t="inlineStr">
+      <c r="A24" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/EDSNBusinessDocumentHeader/Source/SenderID</t>
         </is>
@@ -908,7 +902,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="4" t="inlineStr">
+      <c r="A25" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/Measurement_Series/mRID</t>
         </is>
@@ -925,7 +919,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="4" t="inlineStr">
+      <c r="A26" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/Measurement_Series/product</t>
         </is>
@@ -942,7 +936,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="4" t="inlineStr">
+      <c r="A27" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/Measurement_Series/referenceRevisionRequest_mRID</t>
         </is>
@@ -959,7 +953,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="4" t="inlineStr">
+      <c r="A28" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/Measurement_Series/MarketEvaluationPoint/mRID</t>
         </is>
@@ -976,7 +970,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="4" t="inlineStr">
+      <c r="A29" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/Measurement_Series/MarketParticipant/mRID</t>
         </is>
@@ -993,7 +987,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="4" t="inlineStr">
+      <c r="A30" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/Measurement_Series/MarketParticipant/MarketRole/type</t>
         </is>
@@ -1010,7 +1004,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="4" t="inlineStr">
+      <c r="A31" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/Measurement_Series/Domain/mRID</t>
         </is>
@@ -1027,7 +1021,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="4" t="inlineStr">
+      <c r="A32" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/Measurement_Series/Domain/sourceDomain</t>
         </is>
@@ -1044,7 +1038,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="4" t="inlineStr">
+      <c r="A33" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/Measurement_Series/Domain/sinkDomain</t>
         </is>
@@ -1061,7 +1055,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="4" t="inlineStr">
+      <c r="A34" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/Measurement_Series/DateAndOrTime/startDateTime</t>
         </is>
@@ -1078,7 +1072,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="4" t="inlineStr">
+      <c r="A35" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/Measurement_Series/DateAndOrTime/endDateTime</t>
         </is>
@@ -1095,7 +1089,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="4" t="inlineStr">
+      <c r="A36" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/Measurement_Series/Detail_Series/resolution</t>
         </is>
@@ -1112,7 +1106,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="4" t="inlineStr">
+      <c r="A37" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/Measurement_Series/Detail_Series/Product/identification</t>
         </is>
@@ -1129,7 +1123,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="4" t="inlineStr">
+      <c r="A38" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/Measurement_Series/Detail_Series/Product/measureUnit</t>
         </is>
@@ -1146,7 +1140,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="4" t="inlineStr">
+      <c r="A39" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/Measurement_Series/Detail_Series/FlowDirection/direction</t>
         </is>
@@ -1163,7 +1157,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="4" t="inlineStr">
+      <c r="A40" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/Measurement_Series/Detail_Series/Point/position</t>
         </is>
@@ -1180,7 +1174,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="4" t="inlineStr">
+      <c r="A41" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/Measurement_Series/Detail_Series/Point/quantity</t>
         </is>
@@ -1197,7 +1191,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="4" t="inlineStr">
+      <c r="A42" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/Measurement_Series/Detail_Series/Point/origin</t>
         </is>
@@ -1214,7 +1208,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="4" t="inlineStr">
+      <c r="A43" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/Measurement_Series/Detail_Series/Point/validationStatus</t>
         </is>
@@ -1231,7 +1225,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="4" t="inlineStr">
+      <c r="A44" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/Measurement_Series/Detail_Series/Point/repairMethod</t>
         </is>
@@ -1248,7 +1242,7 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="4" t="inlineStr">
+      <c r="A45" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/Measurement_Series/RestVolume_Quantity/quantity</t>
         </is>
@@ -1265,7 +1259,7 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="4" t="inlineStr">
+      <c r="A46" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/Measurement_Series/RestVolume_Quantity/Product</t>
         </is>
@@ -1282,7 +1276,7 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="4" t="inlineStr">
+      <c r="A47" s="2" t="inlineStr">
         <is>
           <t>MeasurementSeriesNotification/Measurement_Series/RestVolume_Quantity/FlowDirection</t>
         </is>
@@ -1299,17 +1293,17 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="4" t="inlineStr"/>
+      <c r="A48" s="2" t="inlineStr"/>
     </row>
     <row r="49">
-      <c r="A49" s="4" t="inlineStr">
+      <c r="A49" s="2" t="inlineStr">
         <is>
           <t>info para json</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="4" t="inlineStr">
+      <c r="A50" s="2" t="inlineStr">
         <is>
           <t>message path</t>
         </is>
@@ -1326,7 +1320,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="4" t="inlineStr">
+      <c r="A51" s="2" t="inlineStr">
         <is>
           <t>message name</t>
         </is>
@@ -1343,7 +1337,7 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="4" t="inlineStr">
+      <c r="A52" s="2" t="inlineStr">
         <is>
           <t>values file</t>
         </is>
@@ -1360,7 +1354,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="4" t="inlineStr">
+      <c r="A53" s="2" t="inlineStr">
         <is>
           <t>error code</t>
         </is>
@@ -1377,7 +1371,7 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="4" t="inlineStr">
+      <c r="A54" s="2" t="inlineStr">
         <is>
           <t>Message ID</t>
         </is>
@@ -1394,7 +1388,7 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="4" t="inlineStr">
+      <c r="A55" s="2" t="inlineStr">
         <is>
           <t>startDate</t>
         </is>
@@ -1411,7 +1405,7 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="4" t="inlineStr">
+      <c r="A56" s="2" t="inlineStr">
         <is>
           <t>endDate</t>
         </is>
@@ -1428,7 +1422,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="4" t="inlineStr">
+      <c r="A57" s="2" t="inlineStr">
         <is>
           <t>receiver</t>
         </is>
@@ -1445,7 +1439,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="4" t="inlineStr">
+      <c r="A58" s="2" t="inlineStr">
         <is>
           <t>grid_point</t>
         </is>
@@ -1462,7 +1456,7 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="4" t="inlineStr">
+      <c r="A59" s="2" t="inlineStr">
         <is>
           <t>direction</t>
         </is>
@@ -1479,7 +1473,7 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="4" t="inlineStr">
+      <c r="A60" s="2" t="inlineStr">
         <is>
           <t>timeSeries</t>
         </is>
@@ -1496,14 +1490,14 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="4" t="inlineStr">
+      <c r="A61" s="2" t="inlineStr">
         <is>
           <t>struct</t>
         </is>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="4" t="inlineStr">
+      <c r="A62" s="2" t="inlineStr">
         <is>
           <t>struct_market_paries</t>
         </is>
@@ -1520,7 +1514,7 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="4" t="inlineStr">
+      <c r="A63" s="2" t="inlineStr">
         <is>
           <t>struct_net_areas</t>
         </is>
@@ -1537,7 +1531,7 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="4" t="inlineStr">
+      <c r="A64" s="2" t="inlineStr">
         <is>
           <t>struct_grid_points</t>
         </is>
@@ -1554,7 +1548,7 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="4" t="inlineStr">
+      <c r="A65" s="2" t="inlineStr">
         <is>
           <t>struct_supply_contracts</t>
         </is>
@@ -1571,7 +1565,7 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="4" t="inlineStr">
+      <c r="A66" s="2" t="inlineStr">
         <is>
           <t>struct_connections</t>
         </is>
@@ -1607,17 +1601,17 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>XML ELEMENT PATH</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>DEFAULT VALUES</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Error Message 1</t>
         </is>

</xml_diff>